<commit_message>
sort algorithms and performance comparison data
</commit_message>
<xml_diff>
--- a/SortAlgorithmsPerfComparision.xlsx
+++ b/SortAlgorithmsPerfComparision.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1660" windowWidth="36960" windowHeight="21400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,10 +68,10 @@
     <t>R_1Milion</t>
   </si>
   <si>
-    <t>Num Integers/SortAlgorithm</t>
-  </si>
-  <si>
-    <t>AiHa vs Counting Sort</t>
+    <t>AiHa Sort vs Counting Sort</t>
+  </si>
+  <si>
+    <t>Num Integers/SortAlgorithm (Clicks)</t>
   </si>
 </sst>
 </file>
@@ -246,6 +246,36 @@
             </a:rPr>
             <a:t>Legend</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:latin typeface="Arial" charset="0"/>
+            <a:ea typeface="Arial" charset="0"/>
+            <a:cs typeface="Arial" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Arial" charset="0"/>
+              <a:ea typeface="Arial" charset="0"/>
+              <a:cs typeface="Arial" charset="0"/>
+            </a:rPr>
+            <a:t>The performance numbers in the cells are Clicks (Clock</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:latin typeface="Arial" charset="0"/>
+              <a:ea typeface="Arial" charset="0"/>
+              <a:cs typeface="Arial" charset="0"/>
+            </a:rPr>
+            <a:t> ticks)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:latin typeface="Arial" charset="0"/>
+            <a:ea typeface="Arial" charset="0"/>
+            <a:cs typeface="Arial" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1400">
@@ -631,12 +661,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -646,12 +676,12 @@
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.1640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -681,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">

</xml_diff>